<commit_message>
analisando tr e testando nova tabela de produtos
</commit_message>
<xml_diff>
--- a/entrada.xlsx
+++ b/entrada.xlsx
@@ -25,14 +25,13 @@
     <t xml:space="preserve">Produtos</t>
   </si>
   <si>
-    <t xml:space="preserve">Ultrabook Dell Latitude Core I7 7ª Ger Ddr4 16gb Ssd 512gb</t>
+    <t xml:space="preserve">Ar Condicionado Split Hw On/off Eco Garden Gree 18000 Btus, Quente/Frio, 220V, Monofásico – GWH18QD-D3NNB4B</t>
   </si>
   <si>
-    <t xml:space="preserve">Notebook gamer Acer Aspire Nitro 5 AN515-44 preta e vermelha 15.6", AMD Ryzen 7 4800H 8GB de RAM 512GB SSD, NVIDIA GeForce GTX 1650 144 Hz 1920x1080px Windows 11 Home</t>
+    <t xml:space="preserve">Ventilador de Parede 1 Metro, Com 3 velocidades, Ventisol, 220V</t>
   </si>
   <si>
-    <t xml:space="preserve">Notebook Samsung Intel Core I5-1135g7 8gb 256gb Ssd W11 15,6 Np550xda-kh2br - Cinza Chumbo
-</t>
+    <t xml:space="preserve">Frigobar Midea MRC06B1, 45L, 110V, Branco</t>
   </si>
 </sst>
 </file>
@@ -398,10 +397,10 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="153.32"/>
   </cols>
@@ -421,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>